<commit_message>
Edit Sign_Up test case
</commit_message>
<xml_diff>
--- a/testcase/TestCase.xlsx
+++ b/testcase/TestCase.xlsx
@@ -2,17 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NAM4\LAPTRINHHUONGDOITUONG\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\LESA\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="News" sheetId="1" r:id="rId1"/>
+    <sheet name="Sign_up" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="176">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -383,9 +383,6 @@
     <t xml:space="preserve">Hiển thị message : "Bạn chưa nhập Password!" tại textbox [Username]. </t>
   </si>
   <si>
-    <t xml:space="preserve">Test Conditions  </t>
-  </si>
-  <si>
     <t>TC-24</t>
   </si>
   <si>
@@ -427,9 +424,6 @@
   </si>
   <si>
     <t>TC-50</t>
-  </si>
-  <si>
-    <t>Pass : TC-50</t>
   </si>
   <si>
     <t>1. Không nhập data đến tất cả các trường trên Form.
@@ -666,14 +660,6 @@
 3. Click button [SIGN UP]</t>
   </si>
   <si>
-    <t>Kiểm tra việc thêm mới record [User] thành công trong trường hợp nhập data chứa khoảng trắng hai đầu đến textbox [Password].</t>
-  </si>
-  <si>
-    <t>1. Nhập value = ' TranLeSa  ' đến textbox [Password].
-2. Nhập data hợp lệ đến tất cả các trường còn lại.
-3. Click button [SIGN UP]</t>
-  </si>
-  <si>
     <t>Kiểm tra việc thêm mới record [User] không thành công trong trường hợp không nhập data tại textbox [Nhập lại password].</t>
   </si>
   <si>
@@ -696,40 +682,12 @@
     <t>Hiển thị message : "Mật khẩu không trùng nhau !"</t>
   </si>
   <si>
-    <t>Kiểm tra việc thêm mới record [User] không thành công trong trường hợp nhập data tại textbox [Nhập lại password] trùng với data tại textbox [Password]</t>
-  </si>
-  <si>
     <t>1.Nhập data đến textbox [Nhập lại password] trùng với data [Password].
 2. Nhập data hợp lệ đến tất cả các trường còn lại.
 3. Click button [SIGN UP]</t>
   </si>
   <si>
     <t>TC-34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kiểm tra giao diện khi nhấn 
-nút [connect facebook] </t>
-  </si>
-  <si>
-    <t>1.Click nút 
-[connect facebook]
-2.Bấm OK để lấy thông tin cần thiết từ tài khoản facebook.
-3.Nhập thêm thông tin bắt buộc còn thiếu nếu có
-4.Click button [SIGN UP]</t>
-  </si>
-  <si>
-    <t>TC-35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kiểm tra giao diện khi nhấn 
-nút [connect google] </t>
-  </si>
-  <si>
-    <t>1.Click nút 
-[connect google]
-2.Bấm OK để lấy thông tin cần thiết từ tài khoản google.
-3.Nhập thêm thông tin bắt buộc còn thiếu nếu có
-4.Click button [SIGN UP]</t>
   </si>
   <si>
     <t xml:space="preserve">Click vào [Sign up]
@@ -737,12 +695,42 @@
   </si>
   <si>
     <t>Click vào [Password]</t>
+  </si>
+  <si>
+    <t>Kiểm tra việc thêm mới record [User] thành công trong trường hợp nhập data tại textbox [Nhập lại password] trùng với data tại textbox [Password]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra việc đăng ký thành công trong trường hợp click button [Connect Facebook] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiểm tra việc đăng ký thành công trong trường hợp click button [Connect Google] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click nút 
+[Connect Facebook]
+2. Bấm OK để lấy thông tin cần thiết từ tài khoản facebook.
+3. Bắt đầu truy cập Comment
+</t>
+  </si>
+  <si>
+    <t>1.Click nút 
+[Connect Google]
+2.Bấm OK để lấy thông tin cần thiết từ tài khoản google.
+3. Bắt đầu truy cập Comment</t>
+  </si>
+  <si>
+    <t>Kiểm tra việc thêm mới record [User] thành công trong trường hợp nhập data đúng định dạng đến textbox [Email].</t>
+  </si>
+  <si>
+    <t>1. Nhập value = 'saccawin@.mail.com' đến textbox [Email].
+2. Nhập data hợp lệ đến tất cả các trường còn lại.
+3. Click button [SIGN UP]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -778,12 +766,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -826,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -835,9 +829,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -847,12 +838,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -862,21 +847,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1160,16 +1187,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41:G42"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="23.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="23.140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="24" style="18" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="6" customWidth="1"/>
     <col min="5" max="5" width="34.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" style="1" customWidth="1"/>
@@ -1179,26 +1206,26 @@
   <sheetData>
     <row r="2" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1215,804 +1242,801 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="18">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="236.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="18">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="18">
         <v>3</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="E10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>114</v>
+      <c r="G10" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="18">
         <v>4</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12" s="18">
         <v>5</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="C12" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="A13" s="18">
         <v>6</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+    <row r="14" spans="1:8" s="13" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
         <v>7</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="C14" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="A15" s="18">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="10" t="s">
+      <c r="C15" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
+      <c r="A16" s="18">
         <v>9</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
-        <v>10</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="18">
+        <v>10</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="C17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="E17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
         <v>11</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="10" t="s">
+      <c r="C18" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="A19" s="18">
         <v>12</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="C19" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="A20" s="18">
         <v>13</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="C20" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+      <c r="B21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="13" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="20">
         <v>14</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="C22" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="E22" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G22" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
-        <v>15</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="23" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <v>15</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="C23" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="E23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G23" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+    <row r="24" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
         <v>16</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C24" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="6" t="s">
+      <c r="E24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G24" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+    <row r="25" spans="1:7" s="13" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
         <v>17</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="C25" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="E25" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G25" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+    <row r="26" spans="1:7" s="13" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
         <v>18</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="C26" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="6" t="s">
+      <c r="E26" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G26" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+    <row r="27" spans="1:7" s="13" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
         <v>19</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="C27" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="E27" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G27" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
+    <row r="28" spans="1:7" s="13" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
         <v>20</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="10" t="s">
+      <c r="C28" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="6" t="s">
+      <c r="E28" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G28" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="126" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+    <row r="29" spans="1:7" s="13" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A29" s="20">
         <v>21</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="C29" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="6" t="s">
+      <c r="E29" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G29" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+    <row r="30" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="18">
         <v>22</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="C30" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="6" t="s">
+      <c r="E30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G30" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="126" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
+    <row r="31" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
         <v>23</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="10" t="s">
+      <c r="C31" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="6" t="s">
+      <c r="E31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G31" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+    <row r="32" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="18">
         <v>24</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
+        <v>25</v>
+      </c>
+      <c r="B33" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
-        <v>25</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="C33" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="13" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="20">
+        <v>26</v>
+      </c>
+      <c r="B34" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="6" t="s">
+      <c r="C34" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="G32" s="5" t="s">
+      <c r="E34" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="15" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
-        <v>26</v>
-      </c>
-      <c r="B33" s="1" t="s">
+      <c r="G34" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="13" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="20">
+        <v>27</v>
+      </c>
+      <c r="B35" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="10" t="s">
+      <c r="C35" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="13" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="20">
+        <v>28</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="13" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A37" s="20">
+        <v>29</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="G37" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
-        <v>27</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G34" s="5" t="s">
+    </row>
+    <row r="38" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="20">
+        <v>30</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="A39" s="20">
+        <v>31</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="20">
+        <v>32</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G40" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
-        <v>28</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="G35" s="5" t="s">
+    <row r="41" spans="1:7" ht="126" x14ac:dyDescent="0.25">
+      <c r="A41" s="20">
+        <v>33</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="G41" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="126" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
-        <v>29</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
-        <v>30</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
-        <v>31</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="126" x14ac:dyDescent="0.25">
-      <c r="A39" s="15">
-        <v>32</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="10" t="s">
+    <row r="42" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="20">
+        <v>34</v>
+      </c>
+      <c r="B42" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
-        <v>33</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="126" x14ac:dyDescent="0.25">
-      <c r="A41" s="15">
-        <v>34</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="C42" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" s="18" t="s">
+      <c r="E42" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="G41" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="126" x14ac:dyDescent="0.25">
-      <c r="A42" s="15">
-        <v>35</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="G42" s="5" t="s">
+      <c r="G42" s="4" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2026,240 +2050,278 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="35" style="13" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" style="13" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="25" customWidth="1"/>
+    <col min="4" max="4" width="35" style="28" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="25" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" style="25" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="25" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="25">
+        <v>1</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="C9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="G9" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="C10" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="C9" s="13" t="s">
+      <c r="F10" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C11" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="C10" s="13" t="s">
+      <c r="F11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C12" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="C11" s="13" t="s">
+      <c r="F12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="F13" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="C12" s="13" t="s">
+    </row>
+    <row r="14" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" s="5" t="s">
+      <c r="F14" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="13" t="s">
+      <c r="G15" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="C16" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="C14" s="13" t="s">
+      <c r="F16" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="C17" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="13" t="s">
+      <c r="F17" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="C18" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="C16" s="13" t="s">
+      <c r="F18" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C19" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="C17" s="13" t="s">
+      <c r="F19" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C20" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="C18" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C19" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="G19" s="13" t="s">
+      <c r="F20" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="G20" s="26" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C20" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>